<commit_message>
Fix lab_3, add task_6
</commit_message>
<xml_diff>
--- a/lab_3/solution.xlsx
+++ b/lab_3/solution.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainUser\PycharmProjects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainUser\PycharmProjects\AIS\lab_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28851E73-E33D-4CD3-BEED-A95EA64A76E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6B657A-6AF1-41E6-B1B4-2140707B6329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F503492F-066B-0A45-B6B9-4C824909532E}"/>
+    <workbookView xWindow="-2512" yWindow="8002" windowWidth="19394" windowHeight="11476" xr2:uid="{F503492F-066B-0A45-B6B9-4C824909532E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="14">
   <si>
     <t>класс</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Вариант 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -166,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -184,12 +187,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -402,7 +399,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="7"/>
+            <c:size val="4"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -459,34 +456,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-4.6526315789473687</c:v>
+                  <c:v>4.6526315789473687</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-4.0157894736842108</c:v>
+                  <c:v>4.0157894736842108</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.1689473684210525</c:v>
+                  <c:v>2.1689473684210525</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.19473684210526332</c:v>
+                  <c:v>0.19473684210526332</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.44210526315789456</c:v>
+                  <c:v>-0.44210526315789456</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.8315789473684212</c:v>
+                  <c:v>0.8315789473684212</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.7157894736842103</c:v>
+                  <c:v>-1.7157894736842103</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.352631578947368</c:v>
+                  <c:v>-2.352631578947368</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.2631578947368416</c:v>
+                  <c:v>-4.2631578947368416</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.1736842105263161</c:v>
+                  <c:v>-6.1736842105263161</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -764,34 +761,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-4.6526315789473687</c:v>
+                  <c:v>4.6526315789473687</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-4.0157894736842108</c:v>
+                  <c:v>4.0157894736842108</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.1689473684210525</c:v>
+                  <c:v>2.1689473684210525</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.19473684210526332</c:v>
+                  <c:v>0.19473684210526332</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.44210526315789456</c:v>
+                  <c:v>-0.44210526315789456</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.8315789473684212</c:v>
+                  <c:v>0.8315789473684212</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.7157894736842103</c:v>
+                  <c:v>-1.7157894736842103</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.352631578947368</c:v>
+                  <c:v>-2.352631578947368</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.2631578947368416</c:v>
+                  <c:v>-4.2631578947368416</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.1736842105263161</c:v>
+                  <c:v>-6.1736842105263161</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2532,8 +2529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E67801-61CD-CA47-BD27-20C123FC5A39}">
   <dimension ref="C8:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2543,6 +2540,11 @@
         <v>12</v>
       </c>
     </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="27" spans="3:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="1" t="s">
         <v>0</v>
@@ -2617,8 +2619,8 @@
         <v>-0.4</v>
       </c>
       <c r="O28" s="3">
-        <f>(-0.4+1.21*N28)/0.19</f>
-        <v>-4.6526315789473687</v>
+        <f>(-0.4+1.21*N28)/-0.19</f>
+        <v>4.6526315789473687</v>
       </c>
     </row>
     <row r="29" spans="3:15" ht="17.25" x14ac:dyDescent="0.25">
@@ -2657,8 +2659,8 @@
         <v>-0.3</v>
       </c>
       <c r="O29" s="3">
-        <f t="shared" ref="O29:O37" si="1">(-0.4+1.21*N29)/0.19</f>
-        <v>-4.0157894736842108</v>
+        <f t="shared" ref="O29:O37" si="1">(-0.4+1.21*N29)/-0.19</f>
+        <v>4.0157894736842108</v>
       </c>
     </row>
     <row r="30" spans="3:15" ht="17.25" x14ac:dyDescent="0.25">
@@ -2698,7 +2700,7 @@
       </c>
       <c r="O30" s="3">
         <f t="shared" si="1"/>
-        <v>-2.1689473684210525</v>
+        <v>2.1689473684210525</v>
       </c>
     </row>
     <row r="31" spans="3:15" ht="17.25" x14ac:dyDescent="0.25">
@@ -2738,7 +2740,7 @@
       </c>
       <c r="O31" s="3">
         <f t="shared" si="1"/>
-        <v>-0.19473684210526332</v>
+        <v>0.19473684210526332</v>
       </c>
     </row>
     <row r="32" spans="3:15" ht="17.25" x14ac:dyDescent="0.25">
@@ -2778,7 +2780,7 @@
       </c>
       <c r="O32" s="3">
         <f t="shared" si="1"/>
-        <v>0.44210526315789456</v>
+        <v>-0.44210526315789456</v>
       </c>
     </row>
     <row r="33" spans="3:15" ht="17.25" x14ac:dyDescent="0.25">
@@ -2818,7 +2820,7 @@
       </c>
       <c r="O33" s="3">
         <f t="shared" si="1"/>
-        <v>-0.8315789473684212</v>
+        <v>0.8315789473684212</v>
       </c>
     </row>
     <row r="34" spans="3:15" ht="17.25" x14ac:dyDescent="0.25">
@@ -2858,7 +2860,7 @@
       </c>
       <c r="O34" s="3">
         <f t="shared" si="1"/>
-        <v>1.7157894736842103</v>
+        <v>-1.7157894736842103</v>
       </c>
     </row>
     <row r="35" spans="3:15" ht="17.25" x14ac:dyDescent="0.25">
@@ -2898,7 +2900,7 @@
       </c>
       <c r="O35" s="3">
         <f t="shared" si="1"/>
-        <v>2.352631578947368</v>
+        <v>-2.352631578947368</v>
       </c>
     </row>
     <row r="36" spans="3:15" ht="17.25" x14ac:dyDescent="0.25">
@@ -2938,7 +2940,7 @@
       </c>
       <c r="O36" s="3">
         <f t="shared" si="1"/>
-        <v>4.2631578947368416</v>
+        <v>-4.2631578947368416</v>
       </c>
     </row>
     <row r="37" spans="3:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -2951,7 +2953,7 @@
       <c r="E37" s="6">
         <v>1.3</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="6">
         <v>1.1000000000000001</v>
       </c>
       <c r="G37" s="6">
@@ -2978,7 +2980,7 @@
       </c>
       <c r="O37" s="3">
         <f t="shared" si="1"/>
-        <v>6.1736842105263161</v>
+        <v>-6.1736842105263161</v>
       </c>
     </row>
     <row r="38" spans="3:15" ht="17.25" x14ac:dyDescent="0.25">
@@ -3288,7 +3290,7 @@
       <c r="E47" s="6">
         <v>1.3</v>
       </c>
-      <c r="F47" s="7">
+      <c r="F47" s="6">
         <v>1.1000000000000001</v>
       </c>
       <c r="G47" s="6">
@@ -3618,7 +3620,7 @@
       <c r="E57" s="3">
         <v>1.3</v>
       </c>
-      <c r="F57" s="8">
+      <c r="F57" s="3">
         <v>1.1000000000000001</v>
       </c>
       <c r="G57" s="3">

</xml_diff>